<commit_message>
Reduce red header size by half and add duplicate video prevention
</commit_message>
<xml_diff>
--- a/user_submissions.xlsx
+++ b/user_submissions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="101">
   <si>
     <t>timestamp</t>
   </si>
@@ -28,6 +28,18 @@
     <t>slip_path</t>
   </si>
   <si>
+    <t>video_filename</t>
+  </si>
+  <si>
+    <t>original_filename</t>
+  </si>
+  <si>
+    <t>file_size_mb</t>
+  </si>
+  <si>
+    <t>upload_type</t>
+  </si>
+  <si>
     <t>2025-08-09T11:28:13</t>
   </si>
   <si>
@@ -52,6 +64,90 @@
     <t>2025-08-09T11:48:27</t>
   </si>
   <si>
+    <t>2025-08-10T15:19:09</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:19:18</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:19:22</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:19:51</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:19:54</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:20:25</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:21:28</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:25:53</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:27:42</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:27:57</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:28:01</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:30:51</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:31:03</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:31:09</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:31:51</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:31:54</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:32:10</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:32:34</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:35:59</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:36:05</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:36:11</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:36:41</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:36:45</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:36:51</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:37:55</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:42:27</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:42:52</t>
+  </si>
+  <si>
+    <t>2025-08-10T15:44:25</t>
+  </si>
+  <si>
     <t>Rungnapa</t>
   </si>
   <si>
@@ -61,6 +157,15 @@
     <t>Rung</t>
   </si>
   <si>
+    <t>rung</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
     <t>petchpat@gmail.com</t>
   </si>
   <si>
@@ -70,6 +175,24 @@
     <t>Petchpat@yahoo.com</t>
   </si>
   <si>
+    <t>Video Upload</t>
+  </si>
+  <si>
+    <t>rungnapa@sasin.edu</t>
+  </si>
+  <si>
+    <t>rung@sasin,edu</t>
+  </si>
+  <si>
+    <t>AI@gmail.com</t>
+  </si>
+  <si>
+    <t>ai@yahoo,com</t>
+  </si>
+  <si>
+    <t>AI@sasin.edu</t>
+  </si>
+  <si>
     <t>user_uploads/20250809_112813_Rungnapa.png</t>
   </si>
   <si>
@@ -92,6 +215,108 @@
   </si>
   <si>
     <t>user_uploads/20250809_114827_Rung.png</t>
+  </si>
+  <si>
+    <t>user_uploads/20250810_151909_rung.png</t>
+  </si>
+  <si>
+    <t>user_uploads/20250810_152553_rung.png</t>
+  </si>
+  <si>
+    <t>user_uploads/20250810_152742_rung.png</t>
+  </si>
+  <si>
+    <t>user_uploads/20250810_153051_AI.png</t>
+  </si>
+  <si>
+    <t>user_uploads/20250810_153559_AI.png</t>
+  </si>
+  <si>
+    <t>user_uploads/20250810_154227_AI.png</t>
+  </si>
+  <si>
+    <t>20250810_151918_Felix2.mp4</t>
+  </si>
+  <si>
+    <t>20250810_151922_Felix2.mp4</t>
+  </si>
+  <si>
+    <t>20250810_151951_Felix2.mp4</t>
+  </si>
+  <si>
+    <t>20250810_151954_Felix2.mp4</t>
+  </si>
+  <si>
+    <t>20250810_152025_Felix2.mp4</t>
+  </si>
+  <si>
+    <t>20250810_152128_Felix2.mp4</t>
+  </si>
+  <si>
+    <t>20250810_152757_Khun_A-Standing2.mp4</t>
+  </si>
+  <si>
+    <t>20250810_152801_Khun_A-Standing2.mp4</t>
+  </si>
+  <si>
+    <t>20250810_153103_Christoph.mp4</t>
+  </si>
+  <si>
+    <t>20250810_153109_Christoph.mp4</t>
+  </si>
+  <si>
+    <t>20250810_153151_Christoph.mp4</t>
+  </si>
+  <si>
+    <t>20250810_153154_Christoph.mp4</t>
+  </si>
+  <si>
+    <t>20250810_153210_Christoph.mp4</t>
+  </si>
+  <si>
+    <t>20250810_153234_Christoph.mp4</t>
+  </si>
+  <si>
+    <t>20250810_153605_K.Issara.MOV</t>
+  </si>
+  <si>
+    <t>20250810_153611_K.Issara.MOV</t>
+  </si>
+  <si>
+    <t>20250810_153640_K.Issara.MOV</t>
+  </si>
+  <si>
+    <t>20250810_153645_K.Issara.MOV</t>
+  </si>
+  <si>
+    <t>20250810_153651_K.Issara.MOV</t>
+  </si>
+  <si>
+    <t>20250810_153755_K.Issara.MOV</t>
+  </si>
+  <si>
+    <t>20250810_154252_Movement_in_Communication.mp4</t>
+  </si>
+  <si>
+    <t>20250810_154425_Movement_in_Communication.mp4</t>
+  </si>
+  <si>
+    <t>Felix2.mp4</t>
+  </si>
+  <si>
+    <t>Khun A-Standing2.mp4</t>
+  </si>
+  <si>
+    <t>Christoph.mp4</t>
+  </si>
+  <si>
+    <t>K.Issara.MOV</t>
+  </si>
+  <si>
+    <t>Movement in Communication.mp4</t>
+  </si>
+  <si>
+    <t>video</t>
   </si>
 </sst>
 </file>
@@ -449,13 +674,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,117 +693,719 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11">
+        <v>2.17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12">
+        <v>2.17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13">
+        <v>2.17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G14">
+        <v>2.17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15">
+        <v>2.17</v>
+      </c>
+      <c r="H15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16">
+        <v>2.17</v>
+      </c>
+      <c r="H16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
         <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19">
+        <v>2.84</v>
+      </c>
+      <c r="H19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" t="s">
+        <v>96</v>
+      </c>
+      <c r="G20">
+        <v>2.84</v>
+      </c>
+      <c r="H20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22">
+        <v>5.35</v>
+      </c>
+      <c r="H22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23">
+        <v>5.35</v>
+      </c>
+      <c r="H23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24">
+        <v>5.35</v>
+      </c>
+      <c r="H24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" t="s">
+        <v>97</v>
+      </c>
+      <c r="G25">
+        <v>5.35</v>
+      </c>
+      <c r="H25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" t="s">
+        <v>97</v>
+      </c>
+      <c r="G26">
+        <v>5.35</v>
+      </c>
+      <c r="H26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" t="s">
+        <v>97</v>
+      </c>
+      <c r="G27">
+        <v>5.35</v>
+      </c>
+      <c r="H27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G29">
+        <v>184.56</v>
+      </c>
+      <c r="H29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" t="s">
+        <v>98</v>
+      </c>
+      <c r="G30">
+        <v>184.56</v>
+      </c>
+      <c r="H30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31" t="s">
+        <v>98</v>
+      </c>
+      <c r="G31">
+        <v>184.56</v>
+      </c>
+      <c r="H31" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" t="s">
+        <v>90</v>
+      </c>
+      <c r="F32" t="s">
+        <v>98</v>
+      </c>
+      <c r="G32">
+        <v>184.56</v>
+      </c>
+      <c r="H32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" t="s">
+        <v>98</v>
+      </c>
+      <c r="G33">
+        <v>184.56</v>
+      </c>
+      <c r="H33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" t="s">
+        <v>92</v>
+      </c>
+      <c r="F34" t="s">
+        <v>98</v>
+      </c>
+      <c r="G34">
+        <v>184.56</v>
+      </c>
+      <c r="H34" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36" t="s">
+        <v>99</v>
+      </c>
+      <c r="G36">
+        <v>7.47</v>
+      </c>
+      <c r="H36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" t="s">
+        <v>94</v>
+      </c>
+      <c r="F37" t="s">
+        <v>99</v>
+      </c>
+      <c r="G37">
+        <v>7.47</v>
+      </c>
+      <c r="H37" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix CSV file format to match new enhanced logging structure
</commit_message>
<xml_diff>
--- a/user_submissions.xlsx
+++ b/user_submissions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="112">
   <si>
     <t>timestamp</t>
   </si>
@@ -40,6 +40,12 @@
     <t>upload_type</t>
   </si>
   <si>
+    <t>saved_filename</t>
+  </si>
+  <si>
+    <t>file_path</t>
+  </si>
+  <si>
     <t>2025-08-09T11:28:13</t>
   </si>
   <si>
@@ -148,6 +154,12 @@
     <t>2025-08-10T15:44:25</t>
   </si>
   <si>
+    <t>2025-08-10T16:06:01</t>
+  </si>
+  <si>
+    <t>2025-08-10T16:06:33</t>
+  </si>
+  <si>
     <t>Rungnapa</t>
   </si>
   <si>
@@ -235,6 +247,12 @@
     <t>user_uploads/20250810_154227_AI.png</t>
   </si>
   <si>
+    <t>Video: 20250810_160601_Khun_A-Standing2.mp4</t>
+  </si>
+  <si>
+    <t>Video: 20250810_160633_Pukrirk2.mp4</t>
+  </si>
+  <si>
     <t>20250810_151918_Felix2.mp4</t>
   </si>
   <si>
@@ -316,7 +334,22 @@
     <t>Movement in Communication.mp4</t>
   </si>
   <si>
+    <t>Pukrirk2.mp4</t>
+  </si>
+  <si>
     <t>video</t>
+  </si>
+  <si>
+    <t>20250810_160601_Khun_A-Standing2.mp4</t>
+  </si>
+  <si>
+    <t>20250810_160633_Pukrirk2.mp4</t>
+  </si>
+  <si>
+    <t>user_uploads/20250810_160601_Khun_A-Standing2.mp4</t>
+  </si>
+  <si>
+    <t>user_uploads/20250810_160633_Pukrirk2.mp4</t>
   </si>
 </sst>
 </file>
@@ -674,13 +707,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,707 +738,771 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>50</v>
       </c>
-      <c r="D2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>51</v>
       </c>
-      <c r="D3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>51</v>
       </c>
-      <c r="D4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="G11">
         <v>2.17</v>
       </c>
       <c r="H11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F12" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="G12">
         <v>2.17</v>
       </c>
       <c r="H12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="G13">
         <v>2.17</v>
       </c>
       <c r="H13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="F14" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="G14">
         <v>2.17</v>
       </c>
       <c r="H14" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="F15" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="G15">
         <v>2.17</v>
       </c>
       <c r="H15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="F16" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="G16">
         <v>2.17</v>
       </c>
       <c r="H16" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="F19" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G19">
         <v>2.84</v>
       </c>
       <c r="H19" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F20" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G20">
         <v>2.84</v>
       </c>
       <c r="H20" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F22" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G22">
         <v>5.35</v>
       </c>
       <c r="H22" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E23" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="F23" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G23">
         <v>5.35</v>
       </c>
       <c r="H23" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E24" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F24" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G24">
         <v>5.35</v>
       </c>
       <c r="H24" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="F25" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G25">
         <v>5.35</v>
       </c>
       <c r="H25" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E26" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F26" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G26">
         <v>5.35</v>
       </c>
       <c r="H26" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E27" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F27" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G27">
         <v>5.35</v>
       </c>
       <c r="H27" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D28" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E29" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F29" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="G29">
         <v>184.56</v>
       </c>
       <c r="H29" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E30" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="F30" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="G30">
         <v>184.56</v>
       </c>
       <c r="H30" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E31" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="F31" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="G31">
         <v>184.56</v>
       </c>
       <c r="H31" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E32" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="F32" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="G32">
         <v>184.56</v>
       </c>
       <c r="H32" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E33" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="F33" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="G33">
         <v>184.56</v>
       </c>
       <c r="H33" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E34" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F34" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="G34">
         <v>184.56</v>
       </c>
       <c r="H34" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D35" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E36" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F36" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="G36">
         <v>7.47</v>
       </c>
       <c r="H36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" t="s">
-        <v>53</v>
-      </c>
-      <c r="E37" t="s">
-        <v>94</v>
-      </c>
       <c r="F37" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="G37">
         <v>7.47</v>
       </c>
       <c r="H37" t="s">
-        <v>100</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" t="s">
+        <v>77</v>
+      </c>
+      <c r="F38" t="s">
+        <v>102</v>
+      </c>
+      <c r="G38">
+        <v>2.84</v>
+      </c>
+      <c r="H38" t="s">
+        <v>107</v>
+      </c>
+      <c r="I38" t="s">
+        <v>108</v>
+      </c>
+      <c r="J38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" t="s">
+        <v>106</v>
+      </c>
+      <c r="G39">
+        <v>3.9</v>
+      </c>
+      <c r="H39" t="s">
+        <v>107</v>
+      </c>
+      <c r="I39" t="s">
+        <v>109</v>
+      </c>
+      <c r="J39" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>